<commit_message>
added working memory benchmarks
</commit_message>
<xml_diff>
--- a/gonomics/bedtoolsbedopsIntervalOverlap/analysis/BedtoolsHeatmap.xlsx
+++ b/gonomics/bedtoolsbedopsIntervalOverlap/analysis/BedtoolsHeatmap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raven\Desktop\GOPATH\src\github.com\vertgenlab\manuscripts\gonomicsRelease\benchmarking\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F275AA53-AE0F-43E6-843A-362CE45A54B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5020B7D-E4CE-4C38-88D2-D7400CEF20EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="2" activeTab="5" xr2:uid="{8CC73530-0618-C447-AEBF-F42E17D82D60}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="3" activeTab="7" xr2:uid="{8CC73530-0618-C447-AEBF-F42E17D82D60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,11 @@
     <sheet name="finalRun3" sheetId="4" r:id="rId4"/>
     <sheet name="finalRunMem1" sheetId="8" r:id="rId5"/>
     <sheet name="finalRunMem2" sheetId="9" r:id="rId6"/>
-    <sheet name="rileyTouchup" sheetId="5" r:id="rId7"/>
-    <sheet name="ForPdf" sheetId="7" r:id="rId8"/>
-    <sheet name="Scale" sheetId="6" r:id="rId9"/>
+    <sheet name="finalRunMem3" sheetId="10" r:id="rId7"/>
+    <sheet name="finalRunMem4" sheetId="11" r:id="rId8"/>
+    <sheet name="rileyTouchup" sheetId="5" r:id="rId9"/>
+    <sheet name="ForPdf" sheetId="7" r:id="rId10"/>
+    <sheet name="Scale" sheetId="6" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">finalRun1!$A$1:$D$1561</definedName>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1739" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="53">
   <si>
     <t>a</t>
   </si>
@@ -901,6 +903,10 @@
     <xf numFmtId="2" fontId="7" fillId="62" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="7" fillId="63" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -918,10 +924,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1731,12 +1733,12 @@
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="74" t="s">
+      <c r="N15" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="O15" s="74"/>
-      <c r="P15" s="74"/>
-      <c r="Q15" s="74"/>
+      <c r="O15" s="76"/>
+      <c r="P15" s="76"/>
+      <c r="Q15" s="76"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A16">
@@ -1803,7 +1805,7 @@
         <f>AVERAGE(E17:E19)</f>
         <v>1.6513290133288994</v>
       </c>
-      <c r="L17" s="75" t="s">
+      <c r="L17" s="77" t="s">
         <v>7</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -1839,7 +1841,7 @@
       <c r="G18">
         <v>100000</v>
       </c>
-      <c r="L18" s="75"/>
+      <c r="L18" s="77"/>
       <c r="M18" s="2" t="s">
         <v>8</v>
       </c>
@@ -1875,7 +1877,7 @@
       <c r="G19">
         <v>100000</v>
       </c>
-      <c r="L19" s="75"/>
+      <c r="L19" s="77"/>
       <c r="M19" s="2" t="s">
         <v>9</v>
       </c>
@@ -1917,7 +1919,7 @@
         <f>AVERAGE(E20:E22)</f>
         <v>1.7390558562897536</v>
       </c>
-      <c r="L20" s="75"/>
+      <c r="L20" s="77"/>
       <c r="M20" s="2" t="s">
         <v>10</v>
       </c>
@@ -2234,6 +2236,1155 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8763E6F0-2753-BA49-ABAC-6B89682505E9}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="17" width="6.1875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+    </row>
+    <row r="3" spans="1:19" ht="16.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="79"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+    </row>
+    <row r="4" spans="1:19" ht="16.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="11"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+    </row>
+    <row r="5" spans="1:19" ht="18" x14ac:dyDescent="0.5">
+      <c r="A5" s="11"/>
+      <c r="B5" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="15">
+        <v>1.26</v>
+      </c>
+      <c r="E5" s="16">
+        <v>1.47</v>
+      </c>
+      <c r="F5" s="17">
+        <v>2.58</v>
+      </c>
+      <c r="G5" s="18">
+        <v>2.82</v>
+      </c>
+      <c r="H5" s="19">
+        <v>2.69</v>
+      </c>
+      <c r="I5" s="20">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="21">
+        <v>0.61</v>
+      </c>
+      <c r="M5" s="22">
+        <v>0.82</v>
+      </c>
+      <c r="N5" s="23">
+        <v>1.57</v>
+      </c>
+      <c r="O5" s="24">
+        <v>3</v>
+      </c>
+      <c r="P5" s="20">
+        <v>4.88</v>
+      </c>
+      <c r="Q5" s="20">
+        <v>8.49</v>
+      </c>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+    </row>
+    <row r="6" spans="1:19" ht="18" x14ac:dyDescent="0.5">
+      <c r="A6" s="11"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="E6" s="26">
+        <v>1.41</v>
+      </c>
+      <c r="F6" s="27">
+        <v>2.4</v>
+      </c>
+      <c r="G6" s="28">
+        <v>2.65</v>
+      </c>
+      <c r="H6" s="29">
+        <v>2.99</v>
+      </c>
+      <c r="I6" s="30">
+        <v>3.5</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="31">
+        <v>0.62</v>
+      </c>
+      <c r="M6" s="32">
+        <v>0.73</v>
+      </c>
+      <c r="N6" s="33">
+        <v>1.6</v>
+      </c>
+      <c r="O6" s="34">
+        <v>2.81</v>
+      </c>
+      <c r="P6" s="20">
+        <v>5.13</v>
+      </c>
+      <c r="Q6" s="20">
+        <v>6.04</v>
+      </c>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+    </row>
+    <row r="7" spans="1:19" ht="18" x14ac:dyDescent="0.5">
+      <c r="A7" s="11"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1.27</v>
+      </c>
+      <c r="E7" s="35">
+        <v>1.35</v>
+      </c>
+      <c r="F7" s="36">
+        <v>1.86</v>
+      </c>
+      <c r="G7" s="37">
+        <v>1.79</v>
+      </c>
+      <c r="H7" s="38">
+        <v>3.04</v>
+      </c>
+      <c r="I7" s="39">
+        <v>3.12</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="40">
+        <v>0.43</v>
+      </c>
+      <c r="M7" s="41">
+        <v>0.47</v>
+      </c>
+      <c r="N7" s="42">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="O7" s="43">
+        <v>2.31</v>
+      </c>
+      <c r="P7" s="20">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="Q7" s="20">
+        <v>6.53</v>
+      </c>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+    </row>
+    <row r="8" spans="1:19" ht="18" x14ac:dyDescent="0.5">
+      <c r="A8" s="11"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="44">
+        <v>2</v>
+      </c>
+      <c r="E8" s="45">
+        <v>1.83</v>
+      </c>
+      <c r="F8" s="46">
+        <v>1.4</v>
+      </c>
+      <c r="G8" s="47">
+        <v>0.99</v>
+      </c>
+      <c r="H8" s="48">
+        <v>2.41</v>
+      </c>
+      <c r="I8" s="49">
+        <v>3.3</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="40">
+        <v>0.43</v>
+      </c>
+      <c r="M8" s="50">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="N8" s="51">
+        <v>0.74</v>
+      </c>
+      <c r="O8" s="52">
+        <v>1.63</v>
+      </c>
+      <c r="P8" s="20">
+        <v>5.21</v>
+      </c>
+      <c r="Q8" s="20">
+        <v>7.57</v>
+      </c>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+    </row>
+    <row r="9" spans="1:19" ht="18" x14ac:dyDescent="0.5">
+      <c r="A9" s="11"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="53">
+        <v>2.11</v>
+      </c>
+      <c r="E9" s="54">
+        <v>1.91</v>
+      </c>
+      <c r="F9" s="55">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="G9" s="40">
+        <v>0.43</v>
+      </c>
+      <c r="H9" s="56">
+        <v>0.72</v>
+      </c>
+      <c r="I9" s="57">
+        <v>1.21</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="58">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M9" s="59">
+        <v>0.48</v>
+      </c>
+      <c r="N9" s="60">
+        <v>0.75</v>
+      </c>
+      <c r="O9" s="61">
+        <v>0.78</v>
+      </c>
+      <c r="P9" s="62">
+        <v>2.37</v>
+      </c>
+      <c r="Q9" s="20">
+        <v>6.64</v>
+      </c>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+    </row>
+    <row r="10" spans="1:19" ht="18" x14ac:dyDescent="0.5">
+      <c r="A10" s="11"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="63">
+        <v>2.64</v>
+      </c>
+      <c r="E10" s="64">
+        <v>1.81</v>
+      </c>
+      <c r="F10" s="65">
+        <v>1.33</v>
+      </c>
+      <c r="G10" s="66">
+        <v>0.36</v>
+      </c>
+      <c r="H10" s="67">
+        <v>0.17</v>
+      </c>
+      <c r="I10" s="68">
+        <v>0.26</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="69">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M10" s="70">
+        <v>0.73</v>
+      </c>
+      <c r="N10" s="71">
+        <v>0.79</v>
+      </c>
+      <c r="O10" s="72">
+        <v>0.64</v>
+      </c>
+      <c r="P10" s="73">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="Q10" s="20">
+        <v>4.96</v>
+      </c>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+    </row>
+    <row r="11" spans="1:19" ht="18" x14ac:dyDescent="0.5">
+      <c r="A11" s="11"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+    </row>
+    <row r="12" spans="1:19" ht="18.399999999999999" x14ac:dyDescent="0.6">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="81" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" s="81"/>
+      <c r="N12" s="81"/>
+      <c r="O12" s="81"/>
+      <c r="P12" s="81"/>
+      <c r="Q12" s="81"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="D12:I12"/>
+    <mergeCell ref="L12:Q12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="75" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE54DD67-B382-984A-9756-821080AB08D1}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B3:B103"/>
+  <sheetViews>
+    <sheetView zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
+      <selection activeCell="AE87" sqref="AE87"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="2" max="2" width="90.6875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B6" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B7" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B8" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B9" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B10" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B11" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B12" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B13" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B14" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B15" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B16" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B17" s="10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B18" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B19" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B20" s="10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B21" s="10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B22" s="10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B23" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B24" s="10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B25" s="10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B26" s="10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B27" s="10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B28" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B29" s="10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B30" s="10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B31" s="10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B32" s="10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B33" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B34" s="10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B35" s="10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B36" s="10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B37" s="10">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B38" s="10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B39" s="10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B40" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B41" s="10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B42" s="10">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B43" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B44" s="10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B45" s="10">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B46" s="10">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B47" s="10">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B48" s="10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B49" s="10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B50" s="10">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B51" s="10">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B52" s="10">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B53" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B54" s="10">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B55" s="10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B56" s="10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B57" s="10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B58" s="10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B59" s="10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B60" s="10">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B61" s="10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B62" s="10">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B63" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B64" s="10">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B65" s="10">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B66" s="10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B67" s="10">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B68" s="10">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B69" s="10">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B70" s="10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B71" s="10">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B72" s="10">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B73" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B74" s="10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B75" s="10">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B76" s="10">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B77" s="10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B78" s="10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B79" s="10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B80" s="10">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B81" s="10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B82" s="10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B83" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B84" s="10">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B85" s="10">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B86" s="10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B87" s="10">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B88" s="10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B89" s="10">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B90" s="10">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B91" s="10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B92" s="10">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B93" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B94" s="10">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B95" s="10">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B96" s="10">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B97" s="10">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B98" s="10">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B99" s="10">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B100" s="10">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B101" s="10">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B102" s="10">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B103" s="10">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3:B103">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF92D050"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="44" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -31048,14 +32199,14 @@
         <v>19</v>
       </c>
       <c r="J1" s="1"/>
-      <c r="K1" s="74" t="s">
+      <c r="K1" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A2">
@@ -31126,7 +32277,7 @@
         <f t="shared" ref="G3:G37" si="1">E3/D3</f>
         <v>0.61907924076607568</v>
       </c>
-      <c r="I3" s="75" t="s">
+      <c r="I3" s="77" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -31175,7 +32326,7 @@
         <f t="shared" si="1"/>
         <v>0.43366578410912898</v>
       </c>
-      <c r="I4" s="75"/>
+      <c r="I4" s="77"/>
       <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
@@ -31222,7 +32373,7 @@
         <f t="shared" si="1"/>
         <v>0.43415816228596149</v>
       </c>
-      <c r="I5" s="75"/>
+      <c r="I5" s="77"/>
       <c r="J5" s="2" t="s">
         <v>24</v>
       </c>
@@ -31269,7 +32420,7 @@
         <f t="shared" si="1"/>
         <v>0.57182082692359326</v>
       </c>
-      <c r="I6" s="75"/>
+      <c r="I6" s="77"/>
       <c r="J6" s="2" t="s">
         <v>9</v>
       </c>
@@ -31316,7 +32467,7 @@
         <f t="shared" si="1"/>
         <v>0.56730975151328067</v>
       </c>
-      <c r="I7" s="75"/>
+      <c r="I7" s="77"/>
       <c r="J7" s="2" t="s">
         <v>25</v>
       </c>
@@ -31363,7 +32514,7 @@
         <f t="shared" si="1"/>
         <v>0.81678973377506259</v>
       </c>
-      <c r="I8" s="75"/>
+      <c r="I8" s="77"/>
       <c r="J8" s="2" t="s">
         <v>10</v>
       </c>
@@ -31439,14 +32590,14 @@
         <v>20</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="74" t="s">
+      <c r="K10" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="74"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74"/>
-      <c r="P10" s="74"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A11">
@@ -31517,7 +32668,7 @@
         <f t="shared" si="1"/>
         <v>0.48098611109709782</v>
       </c>
-      <c r="I12" s="75" t="s">
+      <c r="I12" s="77" t="s">
         <v>7</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -31566,7 +32717,7 @@
         <f t="shared" si="1"/>
         <v>0.72774144925039641</v>
       </c>
-      <c r="I13" s="75"/>
+      <c r="I13" s="77"/>
       <c r="J13" s="2" t="s">
         <v>8</v>
       </c>
@@ -31613,7 +32764,7 @@
         <f t="shared" si="1"/>
         <v>1.5710371741998712</v>
       </c>
-      <c r="I14" s="75"/>
+      <c r="I14" s="77"/>
       <c r="J14" s="2" t="s">
         <v>24</v>
       </c>
@@ -31660,7 +32811,7 @@
         <f t="shared" si="1"/>
         <v>1.598994797087512</v>
       </c>
-      <c r="I15" s="75"/>
+      <c r="I15" s="77"/>
       <c r="J15" s="2" t="s">
         <v>9</v>
       </c>
@@ -31707,7 +32858,7 @@
         <f t="shared" si="1"/>
         <v>1.1249140123699652</v>
       </c>
-      <c r="I16" s="75"/>
+      <c r="I16" s="77"/>
       <c r="J16" s="2" t="s">
         <v>25</v>
       </c>
@@ -31754,7 +32905,7 @@
         <f t="shared" si="1"/>
         <v>0.73900053840600011</v>
       </c>
-      <c r="I17" s="75"/>
+      <c r="I17" s="77"/>
       <c r="J17" s="2" t="s">
         <v>10</v>
       </c>
@@ -33958,8 +35109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B962EF1-F297-46BE-9361-BD82EAC23158}">
   <dimension ref="A1:S365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="121" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView zoomScale="89" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -34014,14 +35165,14 @@
         <v>47</v>
       </c>
       <c r="M1" s="1"/>
-      <c r="N1" s="74" t="s">
+      <c r="N1" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="74"/>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="81"/>
-      <c r="R1" s="81"/>
-      <c r="S1" s="81"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2">
@@ -34102,7 +35253,7 @@
         <f t="shared" ref="J3:J5" si="1">F3/D3</f>
         <v>0.89317993210109392</v>
       </c>
-      <c r="L3" s="75" t="s">
+      <c r="L3" s="77" t="s">
         <v>7</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -34150,7 +35301,7 @@
         <f t="shared" si="1"/>
         <v>0.71389297156151321</v>
       </c>
-      <c r="L4" s="75"/>
+      <c r="L4" s="77"/>
       <c r="M4" s="2" t="s">
         <v>10</v>
       </c>
@@ -34196,17 +35347,17 @@
         <f t="shared" si="1"/>
         <v>0.85551430696684116</v>
       </c>
-      <c r="L5" s="80"/>
+      <c r="L5" s="74"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="L6" s="9" t="s">
         <v>48</v>
       </c>
       <c r="M6" s="1"/>
-      <c r="N6" s="74" t="s">
+      <c r="N6" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="74"/>
+      <c r="O6" s="76"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="L7" s="1"/>
@@ -34219,7 +35370,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="77" t="s">
         <v>7</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -34233,7 +35384,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="L9" s="75"/>
+      <c r="L9" s="77"/>
       <c r="M9" s="2" t="s">
         <v>10</v>
       </c>
@@ -34245,21 +35396,21 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="17.649999999999999" x14ac:dyDescent="0.5">
-      <c r="L10" s="80"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="81"/>
-      <c r="S10" s="81"/>
+      <c r="L10" s="74"/>
+      <c r="P10" s="75"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="75"/>
+      <c r="S10" s="75"/>
     </row>
     <row r="11" spans="1:19" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="L11" s="9" t="s">
         <v>49</v>
       </c>
       <c r="M11" s="1"/>
-      <c r="N11" s="74" t="s">
+      <c r="N11" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="O11" s="74"/>
+      <c r="O11" s="76"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="L12" s="1"/>
@@ -34272,7 +35423,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="L13" s="75" t="s">
+      <c r="L13" s="77" t="s">
         <v>7</v>
       </c>
       <c r="M13" s="2" t="s">
@@ -34286,7 +35437,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="L14" s="75"/>
+      <c r="L14" s="77"/>
       <c r="M14" s="2" t="s">
         <v>10</v>
       </c>
@@ -34298,17 +35449,17 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="L15" s="80"/>
+      <c r="L15" s="74"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="L16" s="9" t="s">
         <v>50</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="74" t="s">
+      <c r="N16" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="O16" s="74"/>
+      <c r="O16" s="76"/>
     </row>
     <row r="17" spans="12:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="L17" s="1"/>
@@ -34321,7 +35472,7 @@
       </c>
     </row>
     <row r="18" spans="12:15" x14ac:dyDescent="0.5">
-      <c r="L18" s="75" t="s">
+      <c r="L18" s="77" t="s">
         <v>7</v>
       </c>
       <c r="M18" s="2" t="s">
@@ -34335,7 +35486,7 @@
       </c>
     </row>
     <row r="19" spans="12:15" x14ac:dyDescent="0.5">
-      <c r="L19" s="75"/>
+      <c r="L19" s="77"/>
       <c r="M19" s="2" t="s">
         <v>10</v>
       </c>
@@ -34656,6 +35807,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="N11:O11"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="L18:L19"/>
@@ -34663,10 +35815,9 @@
     <mergeCell ref="L13:L14"/>
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N1:O1"/>
   </mergeCells>
-  <conditionalFormatting sqref="N3:O4">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="N3:O4 N8:O9 N13:O14 N18:O19">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0.25"/>
         <cfvo type="num" val="1"/>
@@ -34677,8 +35828,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:O4 N8:O9 N13:O14 N18:O19">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="N3:O4">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0.25"/>
         <cfvo type="num" val="1"/>
@@ -34695,6 +35846,1470 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C02E96-92D4-447C-8BC1-5F3E9E71E054}">
+  <dimension ref="A1:S365"/>
+  <sheetViews>
+    <sheetView zoomScale="63" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="10.3125" customWidth="1"/>
+    <col min="3" max="3" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="22.875" customWidth="1"/>
+    <col min="6" max="6" width="20.25" customWidth="1"/>
+    <col min="7" max="7" width="15.6875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="7.5" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="7.5" style="7" customWidth="1"/>
+    <col min="12" max="12" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.1875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.875" customWidth="1"/>
+    <col min="15" max="15" width="14.4375" customWidth="1"/>
+    <col min="16" max="17" width="32.3125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="4.6875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="3.8125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="17.649999999999999" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="76"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>12638</v>
+      </c>
+      <c r="D2">
+        <f>MAX(12274,12028,12452)</f>
+        <v>12452</v>
+      </c>
+      <c r="E2">
+        <v>12714</v>
+      </c>
+      <c r="F2">
+        <v>12645</v>
+      </c>
+      <c r="G2" s="7">
+        <f>E2/C2</f>
+        <v>1.0060136097483778</v>
+      </c>
+      <c r="H2" s="7">
+        <f>E2/D2</f>
+        <v>1.0210407966591712</v>
+      </c>
+      <c r="I2" s="7">
+        <f>F2/C2</f>
+        <v>1.0005538851084033</v>
+      </c>
+      <c r="J2" s="7">
+        <f>F2/D2</f>
+        <v>1.0154995181496949</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>10000000</v>
+      </c>
+      <c r="C3">
+        <v>12488</v>
+      </c>
+      <c r="D3">
+        <f>MAX(12235,12697,12704)</f>
+        <v>12704</v>
+      </c>
+      <c r="E3">
+        <v>12471</v>
+      </c>
+      <c r="F3">
+        <v>12491</v>
+      </c>
+      <c r="G3" s="7">
+        <f>E3/C3</f>
+        <v>0.99863869314541964</v>
+      </c>
+      <c r="H3" s="7">
+        <f>E3/D3</f>
+        <v>0.98165931989924438</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" ref="I3:I5" si="0">F3/C3</f>
+        <v>1.0002402306213964</v>
+      </c>
+      <c r="J3" s="7">
+        <f t="shared" ref="J3:J5" si="1">F3/D3</f>
+        <v>0.98323362720403018</v>
+      </c>
+      <c r="L3" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <v>10000000</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>69646</v>
+      </c>
+      <c r="D4">
+        <f>MAX(69993,44825,44794)</f>
+        <v>69993</v>
+      </c>
+      <c r="E4">
+        <v>37814</v>
+      </c>
+      <c r="F4">
+        <v>63313</v>
+      </c>
+      <c r="G4" s="7">
+        <f>E4/C4</f>
+        <v>0.54294575424288549</v>
+      </c>
+      <c r="H4" s="7">
+        <f>E4/D4</f>
+        <v>0.54025402540254031</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.9090687189501192</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="1"/>
+        <v>0.90456188475990451</v>
+      </c>
+      <c r="L4" s="77"/>
+      <c r="M4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A5">
+        <v>10000000</v>
+      </c>
+      <c r="B5">
+        <v>10000000</v>
+      </c>
+      <c r="C5">
+        <v>82132</v>
+      </c>
+      <c r="D5">
+        <f>MAX(82311,82493,82422)</f>
+        <v>82493</v>
+      </c>
+      <c r="E5">
+        <v>61249</v>
+      </c>
+      <c r="F5">
+        <v>78574</v>
+      </c>
+      <c r="G5" s="7">
+        <f>E5/C5</f>
+        <v>0.74573856718453224</v>
+      </c>
+      <c r="H5" s="7">
+        <f>E5/D5</f>
+        <v>0.7424751191010146</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="0"/>
+        <v>0.9566794915501875</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="1"/>
+        <v>0.95249293879480679</v>
+      </c>
+      <c r="L5" s="74"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="76"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L7" s="1"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L8" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="L9" s="77"/>
+      <c r="M9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" ht="17.649999999999999" x14ac:dyDescent="0.5">
+      <c r="L10" s="74"/>
+      <c r="P10" s="75"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="75"/>
+      <c r="S10" s="75"/>
+    </row>
+    <row r="11" spans="1:19" ht="17.649999999999999" x14ac:dyDescent="0.5">
+      <c r="L11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" s="76"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L12" s="1"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L13" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L14" s="77"/>
+      <c r="M14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L15" s="74"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="O16" s="76"/>
+    </row>
+    <row r="17" spans="12:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L17" s="1"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="12:15" x14ac:dyDescent="0.5">
+      <c r="L18" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="12:15" x14ac:dyDescent="0.5">
+      <c r="L19" s="77"/>
+      <c r="M19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="289" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C289" s="5"/>
+    </row>
+    <row r="290" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C290" s="5"/>
+    </row>
+    <row r="291" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C291" s="5"/>
+    </row>
+    <row r="292" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C292" s="5"/>
+    </row>
+    <row r="293" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C293" s="5"/>
+    </row>
+    <row r="294" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C294" s="5"/>
+    </row>
+    <row r="295" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C295" s="5"/>
+    </row>
+    <row r="296" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C296" s="5"/>
+    </row>
+    <row r="297" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C297" s="5"/>
+    </row>
+    <row r="298" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C298" s="5"/>
+    </row>
+    <row r="299" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C299" s="5"/>
+      <c r="D299" s="5"/>
+      <c r="E299" s="5"/>
+      <c r="F299" s="5"/>
+    </row>
+    <row r="300" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E300" s="5"/>
+      <c r="F300" s="5"/>
+    </row>
+    <row r="301" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E301" s="5"/>
+      <c r="F301" s="5"/>
+    </row>
+    <row r="302" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E302" s="5"/>
+      <c r="F302" s="5"/>
+    </row>
+    <row r="303" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E303" s="5"/>
+      <c r="F303" s="5"/>
+    </row>
+    <row r="304" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E304" s="5"/>
+      <c r="F304" s="5"/>
+    </row>
+    <row r="305" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E305" s="5"/>
+      <c r="F305" s="5"/>
+    </row>
+    <row r="306" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E306" s="5"/>
+      <c r="F306" s="5"/>
+    </row>
+    <row r="307" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E307" s="5"/>
+      <c r="F307" s="5"/>
+    </row>
+    <row r="308" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E308" s="5"/>
+      <c r="F308" s="5"/>
+    </row>
+    <row r="309" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E309" s="5"/>
+      <c r="F309" s="5"/>
+    </row>
+    <row r="311" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E311" s="5"/>
+      <c r="F311" s="5"/>
+    </row>
+    <row r="312" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E312" s="5"/>
+      <c r="F312" s="5"/>
+    </row>
+    <row r="313" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E313" s="5"/>
+      <c r="F313" s="5"/>
+    </row>
+    <row r="314" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E314" s="5"/>
+      <c r="F314" s="5"/>
+    </row>
+    <row r="315" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E315" s="5"/>
+      <c r="F315" s="5"/>
+    </row>
+    <row r="316" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E316" s="5"/>
+      <c r="F316" s="5"/>
+    </row>
+    <row r="317" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E317" s="5"/>
+      <c r="F317" s="5"/>
+    </row>
+    <row r="318" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E318" s="5"/>
+      <c r="F318" s="5"/>
+    </row>
+    <row r="319" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E319" s="5"/>
+      <c r="F319" s="5"/>
+    </row>
+    <row r="320" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E320" s="5"/>
+      <c r="F320" s="5"/>
+    </row>
+    <row r="322" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E322" s="5"/>
+      <c r="F322" s="5"/>
+    </row>
+    <row r="323" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E323" s="5"/>
+      <c r="F323" s="5"/>
+    </row>
+    <row r="324" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E324" s="5"/>
+      <c r="F324" s="5"/>
+    </row>
+    <row r="325" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E325" s="5"/>
+      <c r="F325" s="5"/>
+    </row>
+    <row r="326" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E326" s="5"/>
+      <c r="F326" s="5"/>
+    </row>
+    <row r="327" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E327" s="5"/>
+      <c r="F327" s="5"/>
+    </row>
+    <row r="328" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E328" s="5"/>
+      <c r="F328" s="5"/>
+    </row>
+    <row r="329" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E329" s="5"/>
+      <c r="F329" s="5"/>
+    </row>
+    <row r="330" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E330" s="5"/>
+      <c r="F330" s="5"/>
+    </row>
+    <row r="331" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E331" s="5"/>
+      <c r="F331" s="5"/>
+    </row>
+    <row r="333" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E333" s="5"/>
+      <c r="F333" s="5"/>
+    </row>
+    <row r="334" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E334" s="5"/>
+      <c r="F334" s="5"/>
+    </row>
+    <row r="335" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E335" s="5"/>
+      <c r="F335" s="5"/>
+    </row>
+    <row r="336" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E336" s="5"/>
+      <c r="F336" s="5"/>
+    </row>
+    <row r="337" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E337" s="5"/>
+      <c r="F337" s="5"/>
+    </row>
+    <row r="338" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E338" s="5"/>
+      <c r="F338" s="5"/>
+    </row>
+    <row r="339" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E339" s="5"/>
+      <c r="F339" s="5"/>
+    </row>
+    <row r="340" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E340" s="5"/>
+      <c r="F340" s="5"/>
+    </row>
+    <row r="341" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E341" s="5"/>
+      <c r="F341" s="5"/>
+    </row>
+    <row r="342" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E342" s="5"/>
+      <c r="F342" s="5"/>
+    </row>
+    <row r="344" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C344" s="5"/>
+      <c r="E344" s="5"/>
+      <c r="F344" s="5"/>
+    </row>
+    <row r="345" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C345" s="5"/>
+      <c r="E345" s="5"/>
+      <c r="F345" s="5"/>
+    </row>
+    <row r="346" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C346" s="5"/>
+      <c r="E346" s="5"/>
+      <c r="F346" s="5"/>
+    </row>
+    <row r="347" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C347" s="5"/>
+      <c r="E347" s="5"/>
+      <c r="F347" s="5"/>
+    </row>
+    <row r="348" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C348" s="5"/>
+      <c r="E348" s="5"/>
+      <c r="F348" s="5"/>
+    </row>
+    <row r="349" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C349" s="5"/>
+      <c r="E349" s="5"/>
+      <c r="F349" s="5"/>
+    </row>
+    <row r="350" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C350" s="5"/>
+      <c r="E350" s="5"/>
+      <c r="F350" s="5"/>
+    </row>
+    <row r="351" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C351" s="5"/>
+      <c r="E351" s="5"/>
+      <c r="F351" s="5"/>
+    </row>
+    <row r="352" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C352" s="5"/>
+      <c r="E352" s="5"/>
+      <c r="F352" s="5"/>
+    </row>
+    <row r="353" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C353" s="5"/>
+      <c r="E353" s="5"/>
+      <c r="F353" s="5"/>
+    </row>
+    <row r="354" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C354" s="5"/>
+      <c r="D354" s="5"/>
+      <c r="E354" s="5"/>
+      <c r="F354" s="5"/>
+    </row>
+    <row r="355" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C355" s="5"/>
+      <c r="E355" s="5"/>
+      <c r="F355" s="5"/>
+    </row>
+    <row r="356" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C356" s="5"/>
+      <c r="E356" s="5"/>
+      <c r="F356" s="5"/>
+    </row>
+    <row r="357" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C357" s="5"/>
+      <c r="E357" s="5"/>
+      <c r="F357" s="5"/>
+    </row>
+    <row r="358" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C358" s="5"/>
+      <c r="E358" s="5"/>
+      <c r="F358" s="5"/>
+    </row>
+    <row r="359" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C359" s="5"/>
+      <c r="E359" s="5"/>
+      <c r="F359" s="5"/>
+    </row>
+    <row r="360" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C360" s="5"/>
+      <c r="E360" s="5"/>
+      <c r="F360" s="5"/>
+    </row>
+    <row r="361" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C361" s="5"/>
+      <c r="E361" s="5"/>
+      <c r="F361" s="5"/>
+    </row>
+    <row r="362" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C362" s="5"/>
+      <c r="E362" s="5"/>
+      <c r="F362" s="5"/>
+    </row>
+    <row r="363" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C363" s="5"/>
+      <c r="E363" s="5"/>
+      <c r="F363" s="5"/>
+    </row>
+    <row r="364" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C364" s="5"/>
+      <c r="E364" s="5"/>
+      <c r="F364" s="5"/>
+    </row>
+    <row r="365" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C365" s="5"/>
+      <c r="D365" s="5"/>
+      <c r="E365" s="5"/>
+      <c r="F365" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="L13:L14"/>
+  </mergeCells>
+  <conditionalFormatting sqref="N3:O4 N8:O9 N13:O14 N18:O19">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0.25"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="4"/>
+        <color rgb="FF92D050"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:O4">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0.25"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="4"/>
+        <color rgb="FF92D050"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF231DB-9C48-4EE9-B7D3-4206B8F220B9}">
+  <dimension ref="A1:S365"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="10.3125" customWidth="1"/>
+    <col min="3" max="3" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="22.875" customWidth="1"/>
+    <col min="6" max="6" width="20.25" customWidth="1"/>
+    <col min="7" max="7" width="15.6875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="7.5" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="7.5" style="7" customWidth="1"/>
+    <col min="12" max="12" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.1875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.875" customWidth="1"/>
+    <col min="15" max="15" width="14.4375" customWidth="1"/>
+    <col min="16" max="17" width="32.3125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="4.6875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="3.8125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="17.649999999999999" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="76"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>3848</v>
+      </c>
+      <c r="D2">
+        <f>MAX(1896,1948,16196)</f>
+        <v>16196</v>
+      </c>
+      <c r="E2">
+        <v>13440</v>
+      </c>
+      <c r="F2">
+        <v>13268</v>
+      </c>
+      <c r="G2" s="7">
+        <f>E2/C2</f>
+        <v>3.4927234927234929</v>
+      </c>
+      <c r="H2" s="7">
+        <f>E2/D2</f>
+        <v>0.82983452704371452</v>
+      </c>
+      <c r="I2" s="7">
+        <f>F2/C2</f>
+        <v>3.4480249480249481</v>
+      </c>
+      <c r="J2" s="7">
+        <f>F2/D2</f>
+        <v>0.81921462089404795</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>10000000</v>
+      </c>
+      <c r="C3">
+        <v>4152</v>
+      </c>
+      <c r="D3">
+        <f>MAX(1952,249416,16356)</f>
+        <v>249416</v>
+      </c>
+      <c r="E3">
+        <v>18120</v>
+      </c>
+      <c r="F3">
+        <v>19244</v>
+      </c>
+      <c r="G3" s="7">
+        <f>E3/C3</f>
+        <v>4.3641618497109826</v>
+      </c>
+      <c r="H3" s="7">
+        <f>E3/D3</f>
+        <v>7.2649709721910385E-2</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" ref="I3:I5" si="0">F3/C3</f>
+        <v>4.6348747591522157</v>
+      </c>
+      <c r="J3" s="7">
+        <f t="shared" ref="J3:J5" si="1">F3/D3</f>
+        <v>7.7156236969560893E-2</v>
+      </c>
+      <c r="L3" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="O3" s="3">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <v>10000000</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>3362556</v>
+      </c>
+      <c r="D4">
+        <f>MAX(247224,1944,16356)</f>
+        <v>247224</v>
+      </c>
+      <c r="E4">
+        <v>13052600</v>
+      </c>
+      <c r="F4">
+        <v>13271332</v>
+      </c>
+      <c r="G4" s="7">
+        <f>E4/C4</f>
+        <v>3.8817494786703923</v>
+      </c>
+      <c r="H4" s="7">
+        <f>E4/D4</f>
+        <v>52.796654046532701</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="0"/>
+        <v>3.9467988042429627</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="1"/>
+        <v>53.681406335954435</v>
+      </c>
+      <c r="L4" s="77"/>
+      <c r="M4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="3">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="O4" s="3">
+        <v>4.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A5">
+        <v>10000000</v>
+      </c>
+      <c r="B5">
+        <v>10000000</v>
+      </c>
+      <c r="C5">
+        <v>3362568</v>
+      </c>
+      <c r="D5">
+        <f>MAX(250160,248692,16356)</f>
+        <v>250160</v>
+      </c>
+      <c r="E5">
+        <v>14986164</v>
+      </c>
+      <c r="F5">
+        <v>15039484</v>
+      </c>
+      <c r="G5" s="7">
+        <f>E5/C5</f>
+        <v>4.4567616179063148</v>
+      </c>
+      <c r="H5" s="7">
+        <f>E5/D5</f>
+        <v>59.906315957787015</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="0"/>
+        <v>4.4726185463015176</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="1"/>
+        <v>60.119459545890628</v>
+      </c>
+      <c r="L5" s="74"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="76"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L7" s="1"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L8" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.83</v>
+      </c>
+      <c r="O8" s="3">
+        <v>52.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="L9" s="77"/>
+      <c r="M9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O9" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="17.649999999999999" x14ac:dyDescent="0.5">
+      <c r="L10" s="74"/>
+      <c r="P10" s="75"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="75"/>
+      <c r="S10" s="75"/>
+    </row>
+    <row r="11" spans="1:19" ht="17.649999999999999" x14ac:dyDescent="0.5">
+      <c r="L11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" s="76"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L12" s="1"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L13" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13" s="3">
+        <v>3.45</v>
+      </c>
+      <c r="O13" s="3">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L14" s="77"/>
+      <c r="M14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="3">
+        <v>4.63</v>
+      </c>
+      <c r="O14" s="3">
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L15" s="74"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="O16" s="76"/>
+    </row>
+    <row r="17" spans="12:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L17" s="1"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="12:15" x14ac:dyDescent="0.5">
+      <c r="L18" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="O18" s="3">
+        <v>53.7</v>
+      </c>
+    </row>
+    <row r="19" spans="12:15" x14ac:dyDescent="0.5">
+      <c r="L19" s="77"/>
+      <c r="M19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N19" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="O19" s="3">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="289" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C289" s="5"/>
+    </row>
+    <row r="290" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C290" s="5"/>
+    </row>
+    <row r="291" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C291" s="5"/>
+    </row>
+    <row r="292" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C292" s="5"/>
+    </row>
+    <row r="293" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C293" s="5"/>
+    </row>
+    <row r="294" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C294" s="5"/>
+    </row>
+    <row r="295" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C295" s="5"/>
+    </row>
+    <row r="296" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C296" s="5"/>
+    </row>
+    <row r="297" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C297" s="5"/>
+    </row>
+    <row r="298" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C298" s="5"/>
+    </row>
+    <row r="299" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C299" s="5"/>
+      <c r="D299" s="5"/>
+      <c r="E299" s="5"/>
+      <c r="F299" s="5"/>
+    </row>
+    <row r="300" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E300" s="5"/>
+      <c r="F300" s="5"/>
+    </row>
+    <row r="301" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E301" s="5"/>
+      <c r="F301" s="5"/>
+    </row>
+    <row r="302" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E302" s="5"/>
+      <c r="F302" s="5"/>
+    </row>
+    <row r="303" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E303" s="5"/>
+      <c r="F303" s="5"/>
+    </row>
+    <row r="304" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E304" s="5"/>
+      <c r="F304" s="5"/>
+    </row>
+    <row r="305" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E305" s="5"/>
+      <c r="F305" s="5"/>
+    </row>
+    <row r="306" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E306" s="5"/>
+      <c r="F306" s="5"/>
+    </row>
+    <row r="307" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E307" s="5"/>
+      <c r="F307" s="5"/>
+    </row>
+    <row r="308" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E308" s="5"/>
+      <c r="F308" s="5"/>
+    </row>
+    <row r="309" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E309" s="5"/>
+      <c r="F309" s="5"/>
+    </row>
+    <row r="311" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E311" s="5"/>
+      <c r="F311" s="5"/>
+    </row>
+    <row r="312" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E312" s="5"/>
+      <c r="F312" s="5"/>
+    </row>
+    <row r="313" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E313" s="5"/>
+      <c r="F313" s="5"/>
+    </row>
+    <row r="314" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E314" s="5"/>
+      <c r="F314" s="5"/>
+    </row>
+    <row r="315" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E315" s="5"/>
+      <c r="F315" s="5"/>
+    </row>
+    <row r="316" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E316" s="5"/>
+      <c r="F316" s="5"/>
+    </row>
+    <row r="317" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E317" s="5"/>
+      <c r="F317" s="5"/>
+    </row>
+    <row r="318" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E318" s="5"/>
+      <c r="F318" s="5"/>
+    </row>
+    <row r="319" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E319" s="5"/>
+      <c r="F319" s="5"/>
+    </row>
+    <row r="320" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E320" s="5"/>
+      <c r="F320" s="5"/>
+    </row>
+    <row r="322" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E322" s="5"/>
+      <c r="F322" s="5"/>
+    </row>
+    <row r="323" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E323" s="5"/>
+      <c r="F323" s="5"/>
+    </row>
+    <row r="324" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E324" s="5"/>
+      <c r="F324" s="5"/>
+    </row>
+    <row r="325" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E325" s="5"/>
+      <c r="F325" s="5"/>
+    </row>
+    <row r="326" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E326" s="5"/>
+      <c r="F326" s="5"/>
+    </row>
+    <row r="327" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E327" s="5"/>
+      <c r="F327" s="5"/>
+    </row>
+    <row r="328" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E328" s="5"/>
+      <c r="F328" s="5"/>
+    </row>
+    <row r="329" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E329" s="5"/>
+      <c r="F329" s="5"/>
+    </row>
+    <row r="330" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E330" s="5"/>
+      <c r="F330" s="5"/>
+    </row>
+    <row r="331" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E331" s="5"/>
+      <c r="F331" s="5"/>
+    </row>
+    <row r="333" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E333" s="5"/>
+      <c r="F333" s="5"/>
+    </row>
+    <row r="334" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E334" s="5"/>
+      <c r="F334" s="5"/>
+    </row>
+    <row r="335" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E335" s="5"/>
+      <c r="F335" s="5"/>
+    </row>
+    <row r="336" spans="5:6" x14ac:dyDescent="0.5">
+      <c r="E336" s="5"/>
+      <c r="F336" s="5"/>
+    </row>
+    <row r="337" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E337" s="5"/>
+      <c r="F337" s="5"/>
+    </row>
+    <row r="338" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E338" s="5"/>
+      <c r="F338" s="5"/>
+    </row>
+    <row r="339" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E339" s="5"/>
+      <c r="F339" s="5"/>
+    </row>
+    <row r="340" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E340" s="5"/>
+      <c r="F340" s="5"/>
+    </row>
+    <row r="341" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E341" s="5"/>
+      <c r="F341" s="5"/>
+    </row>
+    <row r="342" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="E342" s="5"/>
+      <c r="F342" s="5"/>
+    </row>
+    <row r="344" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C344" s="5"/>
+      <c r="E344" s="5"/>
+      <c r="F344" s="5"/>
+    </row>
+    <row r="345" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C345" s="5"/>
+      <c r="E345" s="5"/>
+      <c r="F345" s="5"/>
+    </row>
+    <row r="346" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C346" s="5"/>
+      <c r="E346" s="5"/>
+      <c r="F346" s="5"/>
+    </row>
+    <row r="347" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C347" s="5"/>
+      <c r="E347" s="5"/>
+      <c r="F347" s="5"/>
+    </row>
+    <row r="348" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C348" s="5"/>
+      <c r="E348" s="5"/>
+      <c r="F348" s="5"/>
+    </row>
+    <row r="349" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C349" s="5"/>
+      <c r="E349" s="5"/>
+      <c r="F349" s="5"/>
+    </row>
+    <row r="350" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C350" s="5"/>
+      <c r="E350" s="5"/>
+      <c r="F350" s="5"/>
+    </row>
+    <row r="351" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C351" s="5"/>
+      <c r="E351" s="5"/>
+      <c r="F351" s="5"/>
+    </row>
+    <row r="352" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C352" s="5"/>
+      <c r="E352" s="5"/>
+      <c r="F352" s="5"/>
+    </row>
+    <row r="353" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C353" s="5"/>
+      <c r="E353" s="5"/>
+      <c r="F353" s="5"/>
+    </row>
+    <row r="354" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C354" s="5"/>
+      <c r="D354" s="5"/>
+      <c r="E354" s="5"/>
+      <c r="F354" s="5"/>
+    </row>
+    <row r="355" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C355" s="5"/>
+      <c r="E355" s="5"/>
+      <c r="F355" s="5"/>
+    </row>
+    <row r="356" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C356" s="5"/>
+      <c r="E356" s="5"/>
+      <c r="F356" s="5"/>
+    </row>
+    <row r="357" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C357" s="5"/>
+      <c r="E357" s="5"/>
+      <c r="F357" s="5"/>
+    </row>
+    <row r="358" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C358" s="5"/>
+      <c r="E358" s="5"/>
+      <c r="F358" s="5"/>
+    </row>
+    <row r="359" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C359" s="5"/>
+      <c r="E359" s="5"/>
+      <c r="F359" s="5"/>
+    </row>
+    <row r="360" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C360" s="5"/>
+      <c r="E360" s="5"/>
+      <c r="F360" s="5"/>
+    </row>
+    <row r="361" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C361" s="5"/>
+      <c r="E361" s="5"/>
+      <c r="F361" s="5"/>
+    </row>
+    <row r="362" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C362" s="5"/>
+      <c r="E362" s="5"/>
+      <c r="F362" s="5"/>
+    </row>
+    <row r="363" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C363" s="5"/>
+      <c r="E363" s="5"/>
+      <c r="F363" s="5"/>
+    </row>
+    <row r="364" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C364" s="5"/>
+      <c r="E364" s="5"/>
+      <c r="F364" s="5"/>
+    </row>
+    <row r="365" spans="3:6" x14ac:dyDescent="0.5">
+      <c r="C365" s="5"/>
+      <c r="D365" s="5"/>
+      <c r="E365" s="5"/>
+      <c r="F365" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="L13:L14"/>
+  </mergeCells>
+  <conditionalFormatting sqref="N3:O4 N8:O9 N13:O14 N18:O19">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0.25"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="4"/>
+        <color rgb="FF92D050"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:O4">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0.25"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="4"/>
+        <color rgb="FF92D050"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3A15BC-92BB-1B49-8586-3E054857ADD3}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:X397"/>
@@ -34738,22 +37353,22 @@
       </c>
       <c r="I1" s="9"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="76" t="s">
+      <c r="K1" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="S1" s="76" t="s">
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="S1" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="76"/>
-      <c r="X1" s="76"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A2">
@@ -34806,7 +37421,7 @@
         <f t="shared" ref="G3:G37" si="1">E3/D3</f>
         <v>0.61907924076607568</v>
       </c>
-      <c r="I3" s="75" t="s">
+      <c r="I3" s="77" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -34876,7 +37491,7 @@
         <f t="shared" si="1"/>
         <v>0.43366578410912898</v>
       </c>
-      <c r="I4" s="75"/>
+      <c r="I4" s="77"/>
       <c r="J4" s="2" t="s">
         <v>27</v>
       </c>
@@ -34944,7 +37559,7 @@
         <f t="shared" si="1"/>
         <v>0.43415816228596149</v>
       </c>
-      <c r="I5" s="75"/>
+      <c r="I5" s="77"/>
       <c r="J5" s="2" t="s">
         <v>28</v>
       </c>
@@ -35012,7 +37627,7 @@
         <f t="shared" si="1"/>
         <v>0.57182082692359326</v>
       </c>
-      <c r="I6" s="75"/>
+      <c r="I6" s="77"/>
       <c r="J6" s="2" t="s">
         <v>29</v>
       </c>
@@ -35080,7 +37695,7 @@
         <f t="shared" si="1"/>
         <v>0.56730975151328067</v>
       </c>
-      <c r="I7" s="75"/>
+      <c r="I7" s="77"/>
       <c r="J7" s="2" t="s">
         <v>30</v>
       </c>
@@ -35148,7 +37763,7 @@
         <f t="shared" si="1"/>
         <v>0.81678973377506259</v>
       </c>
-      <c r="I8" s="75"/>
+      <c r="I8" s="77"/>
       <c r="J8" s="2" t="s">
         <v>31</v>
       </c>
@@ -35279,22 +37894,22 @@
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="74" t="s">
+      <c r="K10" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="74"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74"/>
-      <c r="P10" s="74"/>
-      <c r="S10" s="74" t="s">
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="S10" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="T10" s="74"/>
-      <c r="U10" s="74"/>
-      <c r="V10" s="74"/>
-      <c r="W10" s="74"/>
-      <c r="X10" s="74"/>
+      <c r="T10" s="76"/>
+      <c r="U10" s="76"/>
+      <c r="V10" s="76"/>
+      <c r="W10" s="76"/>
+      <c r="X10" s="76"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A11">
@@ -36254,1153 +38869,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8763E6F0-2753-BA49-ABAC-6B89682505E9}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:S18"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="17" width="6.1875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-    </row>
-    <row r="3" spans="1:19" ht="16.149999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="77" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="77" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-    </row>
-    <row r="4" spans="1:19" ht="16.149999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="11"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-    </row>
-    <row r="5" spans="1:19" ht="18" x14ac:dyDescent="0.5">
-      <c r="A5" s="11"/>
-      <c r="B5" s="78" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="15">
-        <v>1.26</v>
-      </c>
-      <c r="E5" s="16">
-        <v>1.47</v>
-      </c>
-      <c r="F5" s="17">
-        <v>2.58</v>
-      </c>
-      <c r="G5" s="18">
-        <v>2.82</v>
-      </c>
-      <c r="H5" s="19">
-        <v>2.69</v>
-      </c>
-      <c r="I5" s="20">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="21">
-        <v>0.61</v>
-      </c>
-      <c r="M5" s="22">
-        <v>0.82</v>
-      </c>
-      <c r="N5" s="23">
-        <v>1.57</v>
-      </c>
-      <c r="O5" s="24">
-        <v>3</v>
-      </c>
-      <c r="P5" s="20">
-        <v>4.88</v>
-      </c>
-      <c r="Q5" s="20">
-        <v>8.49</v>
-      </c>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-    </row>
-    <row r="6" spans="1:19" ht="18" x14ac:dyDescent="0.5">
-      <c r="A6" s="11"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="E6" s="26">
-        <v>1.41</v>
-      </c>
-      <c r="F6" s="27">
-        <v>2.4</v>
-      </c>
-      <c r="G6" s="28">
-        <v>2.65</v>
-      </c>
-      <c r="H6" s="29">
-        <v>2.99</v>
-      </c>
-      <c r="I6" s="30">
-        <v>3.5</v>
-      </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="31">
-        <v>0.62</v>
-      </c>
-      <c r="M6" s="32">
-        <v>0.73</v>
-      </c>
-      <c r="N6" s="33">
-        <v>1.6</v>
-      </c>
-      <c r="O6" s="34">
-        <v>2.81</v>
-      </c>
-      <c r="P6" s="20">
-        <v>5.13</v>
-      </c>
-      <c r="Q6" s="20">
-        <v>6.04</v>
-      </c>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-    </row>
-    <row r="7" spans="1:19" ht="18" x14ac:dyDescent="0.5">
-      <c r="A7" s="11"/>
-      <c r="B7" s="78"/>
-      <c r="C7" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="15">
-        <v>1.27</v>
-      </c>
-      <c r="E7" s="35">
-        <v>1.35</v>
-      </c>
-      <c r="F7" s="36">
-        <v>1.86</v>
-      </c>
-      <c r="G7" s="37">
-        <v>1.79</v>
-      </c>
-      <c r="H7" s="38">
-        <v>3.04</v>
-      </c>
-      <c r="I7" s="39">
-        <v>3.12</v>
-      </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="40">
-        <v>0.43</v>
-      </c>
-      <c r="M7" s="41">
-        <v>0.47</v>
-      </c>
-      <c r="N7" s="42">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="O7" s="43">
-        <v>2.31</v>
-      </c>
-      <c r="P7" s="20">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="Q7" s="20">
-        <v>6.53</v>
-      </c>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-    </row>
-    <row r="8" spans="1:19" ht="18" x14ac:dyDescent="0.5">
-      <c r="A8" s="11"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="44">
-        <v>2</v>
-      </c>
-      <c r="E8" s="45">
-        <v>1.83</v>
-      </c>
-      <c r="F8" s="46">
-        <v>1.4</v>
-      </c>
-      <c r="G8" s="47">
-        <v>0.99</v>
-      </c>
-      <c r="H8" s="48">
-        <v>2.41</v>
-      </c>
-      <c r="I8" s="49">
-        <v>3.3</v>
-      </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="L8" s="40">
-        <v>0.43</v>
-      </c>
-      <c r="M8" s="50">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="N8" s="51">
-        <v>0.74</v>
-      </c>
-      <c r="O8" s="52">
-        <v>1.63</v>
-      </c>
-      <c r="P8" s="20">
-        <v>5.21</v>
-      </c>
-      <c r="Q8" s="20">
-        <v>7.57</v>
-      </c>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-    </row>
-    <row r="9" spans="1:19" ht="18" x14ac:dyDescent="0.5">
-      <c r="A9" s="11"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="53">
-        <v>2.11</v>
-      </c>
-      <c r="E9" s="54">
-        <v>1.91</v>
-      </c>
-      <c r="F9" s="55">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="G9" s="40">
-        <v>0.43</v>
-      </c>
-      <c r="H9" s="56">
-        <v>0.72</v>
-      </c>
-      <c r="I9" s="57">
-        <v>1.21</v>
-      </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="L9" s="58">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="M9" s="59">
-        <v>0.48</v>
-      </c>
-      <c r="N9" s="60">
-        <v>0.75</v>
-      </c>
-      <c r="O9" s="61">
-        <v>0.78</v>
-      </c>
-      <c r="P9" s="62">
-        <v>2.37</v>
-      </c>
-      <c r="Q9" s="20">
-        <v>6.64</v>
-      </c>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-    </row>
-    <row r="10" spans="1:19" ht="18" x14ac:dyDescent="0.5">
-      <c r="A10" s="11"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="63">
-        <v>2.64</v>
-      </c>
-      <c r="E10" s="64">
-        <v>1.81</v>
-      </c>
-      <c r="F10" s="65">
-        <v>1.33</v>
-      </c>
-      <c r="G10" s="66">
-        <v>0.36</v>
-      </c>
-      <c r="H10" s="67">
-        <v>0.17</v>
-      </c>
-      <c r="I10" s="68">
-        <v>0.26</v>
-      </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="L10" s="69">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="M10" s="70">
-        <v>0.73</v>
-      </c>
-      <c r="N10" s="71">
-        <v>0.79</v>
-      </c>
-      <c r="O10" s="72">
-        <v>0.64</v>
-      </c>
-      <c r="P10" s="73">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="Q10" s="20">
-        <v>4.96</v>
-      </c>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-    </row>
-    <row r="11" spans="1:19" ht="18" x14ac:dyDescent="0.5">
-      <c r="A11" s="11"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="N11" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="O11" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="P11" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q11" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-    </row>
-    <row r="12" spans="1:19" ht="18.399999999999999" x14ac:dyDescent="0.6">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="79"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="79"/>
-      <c r="I12" s="79"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="M12" s="79"/>
-      <c r="N12" s="79"/>
-      <c r="O12" s="79"/>
-      <c r="P12" s="79"/>
-      <c r="Q12" s="79"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="D12:I12"/>
-    <mergeCell ref="L12:Q12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="75" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE54DD67-B382-984A-9756-821080AB08D1}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="B3:B103"/>
-  <sheetViews>
-    <sheetView zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
-      <selection activeCell="AE87" sqref="AE87"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="2" max="2" width="90.6875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B3" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B5" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B6" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B7" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B8" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B9" s="10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B10" s="10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B11" s="10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B12" s="10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B13" s="10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B14" s="10">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B15" s="10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B16" s="10">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B17" s="10">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B18" s="10">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B19" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B20" s="10">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B21" s="10">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B22" s="10">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B23" s="10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B24" s="10">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B25" s="10">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B26" s="10">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B27" s="10">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B28" s="10">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B29" s="10">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B30" s="10">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B31" s="10">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B32" s="10">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B33" s="10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B34" s="10">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B35" s="10">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B36" s="10">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B37" s="10">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B38" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B39" s="10">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B40" s="10">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B41" s="10">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B42" s="10">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B43" s="10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B44" s="10">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B45" s="10">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B46" s="10">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B47" s="10">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B48" s="10">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B49" s="10">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B50" s="10">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B51" s="10">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B52" s="10">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B53" s="10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B54" s="10">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B55" s="10">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B56" s="10">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B57" s="10">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B58" s="10">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B59" s="10">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B60" s="10">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B61" s="10">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B62" s="10">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B63" s="10">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B64" s="10">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B65" s="10">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B66" s="10">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B67" s="10">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B68" s="10">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B69" s="10">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B70" s="10">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B71" s="10">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B72" s="10">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B73" s="10">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B74" s="10">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B75" s="10">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B76" s="10">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B77" s="10">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B78" s="10">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B79" s="10">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B80" s="10">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B81" s="10">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B82" s="10">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B83" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B84" s="10">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B85" s="10">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B86" s="10">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B87" s="10">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B88" s="10">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B89" s="10">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B90" s="10">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B91" s="10">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B92" s="10">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B93" s="10">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B94" s="10">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B95" s="10">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B96" s="10">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B97" s="10">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B98" s="10">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B99" s="10">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B100" s="10">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B101" s="10">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B102" s="10">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B103" s="10">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B3:B103">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF92D050"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="44" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>